<commit_message>
Extração de relatórios concluído
</commit_message>
<xml_diff>
--- a/Documentacao/ProductBacklog&BurnDown.xlsx
+++ b/Documentacao/ProductBacklog&BurnDown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LukasReisdeOliveira\Desktop\Facul\AutopecasMcQueen\Documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{799E76DA-1417-4618-917E-7E0FEF51D176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC981CFB-9A58-446E-B0A6-F1BC7089D720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-2400" windowWidth="29040" windowHeight="15720" xr2:uid="{A9A78A5D-B30D-44F0-B5CB-B2B1D3CE7A35}"/>
+    <workbookView xWindow="20370" yWindow="-2400" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{A9A78A5D-B30D-44F0-B5CB-B2B1D3CE7A35}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="4" r:id="rId1"/>
@@ -501,10 +501,10 @@
                   <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>28</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>28</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1847,8 +1847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60974E1B-3A99-44DF-886B-63181F317748}">
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I54" sqref="I54"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D34" sqref="A34:D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2548,12 +2548,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>48</v>
       </c>
       <c r="B35" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="C35" t="s">
         <v>23</v>
@@ -2706,8 +2706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B988CE95-B5BE-457A-8BE6-D647639C07CD}">
   <dimension ref="A2:E17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2959,11 +2959,11 @@
         <v>28</v>
       </c>
       <c r="C15">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E15">
         <v>10</v>
@@ -2981,7 +2981,7 @@
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -2990,7 +2990,7 @@
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17">
         <f>SUM(C4:C16)</f>
-        <v>225</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Documentação atualizada, burnDown e banco de dados
</commit_message>
<xml_diff>
--- a/Documentacao/ProductBacklog&BurnDown.xlsx
+++ b/Documentacao/ProductBacklog&BurnDown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LukasReisdeOliveira\Desktop\Facul\AutopecasMcQueen\Documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC981CFB-9A58-446E-B0A6-F1BC7089D720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08976188-1932-4C0B-B78D-B1CCD5A5D254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-2400" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{A9A78A5D-B30D-44F0-B5CB-B2B1D3CE7A35}"/>
   </bookViews>
@@ -208,7 +208,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -216,13 +216,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -237,19 +257,111 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -501,10 +613,10 @@
                   <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>22</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>22</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -923,7 +1035,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -1489,15 +1601,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>117232</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>139212</xdr:rowOff>
+      <xdr:colOff>50558</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>34437</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>476251</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>24912</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1537,14 +1649,30 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{A8CF0624-9547-42BA-8CE5-855447108A79}" name="Item" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{27872076-ACB9-4388-BF47-24E91B27C8C6}" name="Status" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{F6118AB8-3A98-49B6-BAF6-E971E4C8476E}" name="Prioridade" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{A8CF0624-9547-42BA-8CE5-855447108A79}" name="Item" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{27872076-ACB9-4388-BF47-24E91B27C8C6}" name="Status" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{F6118AB8-3A98-49B6-BAF6-E971E4C8476E}" name="Prioridade" dataDxfId="11"/>
     <tableColumn id="3" xr3:uid="{FF89B8F2-01C0-4FD2-A7CD-39135DA13EC6}" name="Peso (1 a 10)"/>
-    <tableColumn id="4" xr3:uid="{03D0E147-0AC8-4A79-A872-7E0AF4CDCA8A}" name="Tempo Estimado (horas)" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{21F5859F-DF1B-4844-B794-A32662B7741C}" name="Sprint" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{03D0E147-0AC8-4A79-A872-7E0AF4CDCA8A}" name="Tempo Estimado (horas)" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{21F5859F-DF1B-4844-B794-A32662B7741C}" name="Sprint" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{495DC785-E1DB-412A-BC10-229F688C2395}" name="Tabela2" displayName="Tabela2" ref="A2:E17" totalsRowCount="1" headerRowDxfId="6" totalsRowDxfId="1">
+  <autoFilter ref="A2:E16" xr:uid="{495DC785-E1DB-412A-BC10-229F688C2395}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{F2E56BD1-0AB9-4ECF-959D-5E9B29656245}" name="SPRINT" totalsRowDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{DB51CBD9-0D01-444A-8026-53FE5A77C21F}" name="PONTOS TOTAIS" totalsRowDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{5CBCE714-265B-4B32-8222-996E30EB1619}" name="CONCLUÍDO REAL" totalsRowFunction="custom" totalsRowDxfId="0">
+      <totalsRowFormula>SUM(C4:C16)</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{2DE5993D-168D-4D5B-B9E2-6030A488624B}" name="RESTANTE" totalsRowDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{F00D1E94-23F6-4C08-B127-D5848202AE8C}" name="TRAJETÓRIA ESTIMADA " totalsRowDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1847,19 +1975,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60974E1B-3A99-44DF-886B-63181F317748}">
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D34" sqref="A34:D34"/>
+    <sheetView topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.140625" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="13" max="13" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="33.5703125" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -1883,7 +2011,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
@@ -1906,7 +2034,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B3" t="s">
@@ -1928,8 +2056,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:13" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B4" t="s">
@@ -1949,7 +2077,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B5" t="s">
@@ -1969,7 +2097,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B6" t="s">
@@ -1989,7 +2117,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B7" t="s">
@@ -2009,7 +2137,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B8" t="s">
@@ -2029,7 +2157,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B9" t="s">
@@ -2049,7 +2177,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B10" t="s">
@@ -2069,7 +2197,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B11" t="s">
@@ -2089,7 +2217,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B12" t="s">
@@ -2109,7 +2237,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B13" t="s">
@@ -2129,7 +2257,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B14" t="s">
@@ -2149,7 +2277,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B15" t="s">
@@ -2169,7 +2297,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B16" t="s">
@@ -2189,7 +2317,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B17" t="s">
@@ -2209,7 +2337,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B18" t="s">
@@ -2229,7 +2357,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B19" t="s">
@@ -2248,8 +2376,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="20" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B20" t="s">
@@ -2269,7 +2397,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B21" t="s">
@@ -2289,7 +2417,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B22" t="s">
@@ -2309,7 +2437,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B23" t="s">
@@ -2329,7 +2457,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B24" t="s">
@@ -2349,7 +2477,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B25" t="s">
@@ -2369,7 +2497,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B26" t="s">
@@ -2389,7 +2517,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B27" t="s">
@@ -2409,7 +2537,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -2429,7 +2557,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B29" t="s">
@@ -2449,7 +2577,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B30" t="s">
@@ -2469,7 +2597,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B31" t="s">
@@ -2489,7 +2617,7 @@
       </c>
     </row>
     <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B32" t="s">
@@ -2509,7 +2637,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="A33" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B33" t="s">
@@ -2529,11 +2657,11 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="A34" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B34" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="C34" t="s">
         <v>23</v>
@@ -2549,7 +2677,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="A35" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B35" t="s">
@@ -2569,7 +2697,7 @@
       </c>
     </row>
     <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="A36" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B36" t="s">
@@ -2589,7 +2717,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="A37" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B37" t="s">
@@ -2609,7 +2737,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="A38" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B38" t="s">
@@ -2629,7 +2757,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="A39" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B39" t="s">
@@ -2648,12 +2776,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B40" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="C40" t="s">
         <v>13</v>
@@ -2669,7 +2797,7 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="A41" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B41" t="s">
@@ -2695,7 +2823,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
@@ -2707,32 +2835,32 @@
   <dimension ref="A2:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2959,11 +3087,11 @@
         <v>28</v>
       </c>
       <c r="C15">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E15">
         <v>10</v>
@@ -2981,21 +3109,29 @@
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17">
+    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="6">
         <f>SUM(C4:C16)</f>
-        <v>231</v>
-      </c>
+        <v>243</v>
+      </c>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>